<commit_message>
Update training variants list
</commit_message>
<xml_diff>
--- a/training_variants.xlsx
+++ b/training_variants.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epam-my.sharepoint.com/personal/vladimir_kosolapov_epam_com/Documents/grow/data science/deep_learning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladimir_kosolapov/PycharmProjects/object_detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{D845757E-B6DA-1444-A90D-8B1B84C09F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05199500-1898-4F4A-A44E-E0395D446774}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B14AC45-3C7D-CD47-8E14-1A64C82989A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{6A86245E-473A-9842-9040-D34E7A59899B}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>head weights</t>
   </si>
   <si>
-    <t>yolo</t>
-  </si>
-  <si>
     <t>frozen</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>imagenet</t>
+  </si>
+  <si>
+    <t>coco</t>
   </si>
 </sst>
 </file>
@@ -499,19 +499,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -520,7 +520,7 @@
         <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -528,19 +528,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -549,7 +549,7 @@
         <v>7</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -557,10 +557,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -569,7 +569,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -578,7 +578,7 @@
         <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -586,10 +586,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -598,7 +598,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -607,7 +607,7 @@
         <v>7</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -615,10 +615,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -627,7 +627,7 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
@@ -636,7 +636,7 @@
         <v>7</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -647,7 +647,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -656,7 +656,7 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -665,7 +665,7 @@
         <v>7</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -676,7 +676,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -685,7 +685,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
@@ -694,7 +694,7 @@
         <v>7</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -705,7 +705,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -714,7 +714,7 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -723,7 +723,7 @@
         <v>7</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -734,7 +734,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -743,7 +743,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -752,7 +752,7 @@
         <v>7</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -760,19 +760,19 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
@@ -781,7 +781,7 @@
         <v>7</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -792,16 +792,16 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
@@ -810,7 +810,7 @@
         <v>7</v>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -821,16 +821,16 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
@@ -839,27 +839,27 @@
         <v>7</v>
       </c>
       <c r="I13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
       <c r="D14" t="s">
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G14" t="s">
         <v>6</v>
@@ -868,27 +868,27 @@
         <v>7</v>
       </c>
       <c r="I14" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
@@ -897,19 +897,19 @@
         <v>7</v>
       </c>
       <c r="I15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
@@ -917,7 +917,7 @@
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G16" t="s">
         <v>6</v>
@@ -926,19 +926,19 @@
         <v>7</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
@@ -946,7 +946,7 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G17" t="s">
         <v>6</v>
@@ -955,19 +955,19 @@
         <v>7</v>
       </c>
       <c r="I17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
@@ -975,7 +975,7 @@
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
@@ -984,19 +984,19 @@
         <v>7</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
       <c r="D19" t="s">
         <v>6</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G19" t="s">
         <v>6</v>
@@ -1013,19 +1013,19 @@
         <v>7</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
       <c r="D20" t="s">
         <v>6</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s">
         <v>6</v>
@@ -1042,19 +1042,19 @@
         <v>7</v>
       </c>
       <c r="I20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
         <v>6</v>
@@ -1071,18 +1071,18 @@
         <v>7</v>
       </c>
       <c r="I21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -1091,7 +1091,7 @@
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
         <v>6</v>
@@ -1100,27 +1100,27 @@
         <v>7</v>
       </c>
       <c r="I22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
         <v>14</v>
       </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" t="s">
-        <v>15</v>
-      </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
         <v>6</v>
@@ -1129,27 +1129,27 @@
         <v>7</v>
       </c>
       <c r="I23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
         <v>14</v>
       </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>15</v>
-      </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
         <v>6</v>
@@ -1158,27 +1158,27 @@
         <v>7</v>
       </c>
       <c r="I24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E25" t="s">
         <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
         <v>6</v>
@@ -1187,7 +1187,7 @@
         <v>7</v>
       </c>
       <c r="I25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>